<commit_message>
implement parameterization and runmodes for test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -4,38 +4,91 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="test_suite" sheetId="3" r:id="rId1"/>
+    <sheet name="FlightSearchTest" sheetId="4" r:id="rId1"/>
+    <sheet name="SignInTest" sheetId="5" r:id="rId2"/>
+    <sheet name="test_suite" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>fromCity</t>
+  </si>
+  <si>
+    <t>toCity</t>
+  </si>
+  <si>
+    <t>departingDate</t>
+  </si>
+  <si>
+    <t>returningDate</t>
+  </si>
+  <si>
+    <t>adults</t>
+  </si>
+  <si>
+    <t>children</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>passw12rd</t>
+  </si>
+  <si>
+    <t>test2@test</t>
+  </si>
+  <si>
+    <t>testpwd</t>
+  </si>
+  <si>
+    <t>runmode</t>
+  </si>
+  <si>
+    <t>Odessa, Ukraine (ODS-Odessa Intl.)</t>
+  </si>
+  <si>
+    <t>Paris, France (PAR-All Airports)</t>
+  </si>
+  <si>
+    <t>23/06/2018</t>
+  </si>
+  <si>
+    <t>31/07/2018</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>FlightSearchTest</t>
+  </si>
+  <si>
+    <t>SignInTest</t>
+  </si>
   <si>
     <t>TCID</t>
-  </si>
-  <si>
-    <t>Runmode</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>FlightSearchTest</t>
-  </si>
-  <si>
-    <t>SignInTest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -43,6 +96,14 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -62,13 +123,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -361,39 +429,158 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="2" customWidth="1"/>
   </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>